<commit_message>
30% de programa terminado
</commit_message>
<xml_diff>
--- a/Reserva_salida1.xlsx
+++ b/Reserva_salida1.xlsx
@@ -10,8 +10,9 @@
     <sheet name="reserva_total.prn" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Pmax_Pgen.prn" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Mayor_maxima.prn" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Reserva.rep" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Reserva.err" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Menor_optima.prn" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Reserva.rep" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Reserva.err" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
   <si>
     <t>Escenario</t>
   </si>
@@ -42,25 +43,28 @@
     <t>ID</t>
   </si>
   <si>
-    <t>POT_MAX</t>
-  </si>
-  <si>
-    <t>POT_GEN</t>
-  </si>
-  <si>
-    <t>MAX_GEN</t>
-  </si>
-  <si>
-    <t>RESERVA%</t>
-  </si>
-  <si>
-    <t>PORCENTAJE</t>
+    <t>POT_MAX[MW]</t>
+  </si>
+  <si>
+    <t>POT_GEN[MW]</t>
+  </si>
+  <si>
+    <t>MAX_GEN[MW]</t>
+  </si>
+  <si>
+    <t>RESERVA[%]</t>
+  </si>
+  <si>
+    <t>PORCENTAJE[%]</t>
   </si>
   <si>
     <t>DATO</t>
   </si>
   <si>
-    <t>RESOPT</t>
+    <t>RES_OPT[[%]</t>
+  </si>
+  <si>
+    <t>RESOPT[%]</t>
   </si>
 </sst>
 </file>
@@ -517,7 +521,7 @@
         <v>12</v>
       </c>
       <c r="J1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -531,7 +535,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -539,18 +543,36 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -589,4 +611,37 @@
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
informes al 60 %
</commit_message>
<xml_diff>
--- a/Reserva_salida1.xlsx
+++ b/Reserva_salida1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
   <si>
     <t>Escenario</t>
   </si>
@@ -52,16 +52,25 @@
     <t>MAX_GEN[MW]</t>
   </si>
   <si>
-    <t>RESERVA[%]</t>
+    <t>RESERVA_DATO[%]</t>
   </si>
   <si>
     <t>PORCENTAJE[%]</t>
   </si>
   <si>
-    <t>DATO</t>
-  </si>
-  <si>
-    <t>RES_OPT[[%]</t>
+    <t>RES_OPT[%]</t>
+  </si>
+  <si>
+    <t>NUC-A       21.600</t>
+  </si>
+  <si>
+    <t>NUC-B       21.600</t>
+  </si>
+  <si>
+    <t>URBGEN      18.000</t>
+  </si>
+  <si>
+    <t>HYDRO_G     20.000</t>
   </si>
   <si>
     <t>RESOPT[%]</t>
@@ -433,7 +442,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,7 +450,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -469,8 +478,121 @@
       <c r="I1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" t="s">
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="n">
+        <v>101</v>
+      </c>
+      <c r="B2" t="s">
         <v>13</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>944.9999570846558</v>
+      </c>
+      <c r="E2" t="n">
+        <v>749.9989624023438</v>
+      </c>
+      <c r="F2" t="n">
+        <v>195.000994682312</v>
+      </c>
+      <c r="G2" t="n">
+        <v>26.0001685945936</v>
+      </c>
+      <c r="H2" t="n">
+        <v>5</v>
+      </c>
+      <c r="I2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="n">
+        <v>102</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>944.9999570846558</v>
+      </c>
+      <c r="E3" t="n">
+        <v>749.9989624023438</v>
+      </c>
+      <c r="F3" t="n">
+        <v>195.000994682312</v>
+      </c>
+      <c r="G3" t="n">
+        <v>26.0001685945936</v>
+      </c>
+      <c r="H3" t="n">
+        <v>5</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="n">
+        <v>206</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="n">
+        <v>899.9999761581421</v>
+      </c>
+      <c r="E4" t="n">
+        <v>799.9994506835938</v>
+      </c>
+      <c r="F4" t="n">
+        <v>100.0005254745483</v>
+      </c>
+      <c r="G4" t="n">
+        <v>12.50007426743839</v>
+      </c>
+      <c r="H4" t="n">
+        <v>5</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="n">
+        <v>211</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="n">
+        <v>800.4000333607197</v>
+      </c>
+      <c r="E5" t="n">
+        <v>579.9990844726562</v>
+      </c>
+      <c r="F5" t="n">
+        <v>220.4009488880635</v>
+      </c>
+      <c r="G5" t="n">
+        <v>38.00022358456915</v>
+      </c>
+      <c r="H5" t="n">
+        <v>10</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -484,7 +606,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -492,7 +614,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -518,10 +640,123 @@
         <v>11</v>
       </c>
       <c r="I1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="n">
+        <v>101</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>944.9999570846558</v>
+      </c>
+      <c r="E2" t="n">
+        <v>749.9989624023438</v>
+      </c>
+      <c r="F2" t="n">
+        <v>195.000994682312</v>
+      </c>
+      <c r="G2" t="n">
+        <v>26.0001685945936</v>
+      </c>
+      <c r="H2" t="n">
+        <v>5</v>
+      </c>
+      <c r="I2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="n">
+        <v>102</v>
+      </c>
+      <c r="B3" t="s">
         <v>14</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>944.9999570846558</v>
+      </c>
+      <c r="E3" t="n">
+        <v>749.9989624023438</v>
+      </c>
+      <c r="F3" t="n">
+        <v>195.000994682312</v>
+      </c>
+      <c r="G3" t="n">
+        <v>26.0001685945936</v>
+      </c>
+      <c r="H3" t="n">
+        <v>5</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="n">
+        <v>206</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="n">
+        <v>899.9999761581421</v>
+      </c>
+      <c r="E4" t="n">
+        <v>799.9994506835938</v>
+      </c>
+      <c r="F4" t="n">
+        <v>100.0005254745483</v>
+      </c>
+      <c r="G4" t="n">
+        <v>12.50007426743839</v>
+      </c>
+      <c r="H4" t="n">
+        <v>5</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="n">
+        <v>211</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="n">
+        <v>800.4000333607197</v>
+      </c>
+      <c r="E5" t="n">
+        <v>579.9990844726562</v>
+      </c>
+      <c r="F5" t="n">
+        <v>220.4009488880635</v>
+      </c>
+      <c r="G5" t="n">
+        <v>38.00022358456915</v>
+      </c>
+      <c r="H5" t="n">
+        <v>10</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -535,7 +770,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -543,7 +778,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -569,10 +804,7 @@
         <v>11</v>
       </c>
       <c r="I1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>